<commit_message>
keyword list output now a dict. Previous keyword shortlist also now automatically added to new keyword dict output
</commit_message>
<xml_diff>
--- a/dict/prefix.xlsx
+++ b/dict/prefix.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/masayukikishi/Dropbox (Personal)/masayuki_kishi/repositories/create_names_v2/dict/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B935773C-7CEC-7543-A867-50DA56C1BAD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1048F835-CFD5-A849-80C2-02D55450DC30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20720" xr2:uid="{1ED5CA03-E3A9-144B-B2A8-9DA0B6C9D845}"/>
   </bookViews>
@@ -832,7 +832,7 @@
     <t>s</t>
   </si>
   <si>
-    <t>Keyword shortlist (insert "s")</t>
+    <t>shortlist</t>
   </si>
 </sst>
 </file>
@@ -1208,7 +1208,7 @@
   <dimension ref="A1:J65"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="O22" sqref="O22"/>
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>